<commit_message>
Finaly excel with chart
</commit_message>
<xml_diff>
--- a/logs_analysis.xlsx
+++ b/logs_analysis.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dane z logów" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Wykresy" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -122,6 +124,1181 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Ilość błędów w okresie 05-09-2023_17-24-05 - 30-09-2023_15-39-47</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$1:$A$8</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$1:$B$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>rodzaj błędów</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_heating</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$19</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$19</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_motion</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$37:$A$47</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$37:$B$47</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_temperature_sensor</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$55:$A$60</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$55:$B$60</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_door</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$73:$A$83</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$73:$B$83</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_window</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$91:$A$116</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$91:$B$116</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_heating_switch</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$117:$A$127</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$117:$B$127</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_kitchen_switch</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$135:$A$157</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$135:$B$157</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Rodzaj błędów w kolumnie issue_wifi</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Wykresy'!$A$158:$A$162</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Wykresy'!$B$158:$B$162</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Nazwa błędu</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ilość wystąpień</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10080000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>18</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3600000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>36</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12600000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>54</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6300000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>72</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12600000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>90</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="31500000" cy="4500000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>116</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="12600000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>134</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="27720000" cy="3960000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>157</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5040000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="9" name="Chart 9"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55798,4 +56975,982 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B162"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>issue_heating</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>issue_motion</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>issue_temperature_sensor</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>issue_door</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>issue_window</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>issue_heating_switch</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>issue_kitchen_switch</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>issue_wifi</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Nie działa poprawnie</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Nie ma jak działać poprawnie przez umiejscowienie (zdj)</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Nie działa poprawnie ostatnio widziało ruch wczoraj</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Nie wykryła ruchu jak wchodziłem</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Nie wykrywa ruchu</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Nie działa poprawnie nie wykrywa ruchu</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Nie działa poprawnie przez umiejscowienie</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Zewnętrzna czujka ruchu przetestowana</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>nie działa</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Czujka ruchu zewnetrzna</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Nie widzi czujki temperatury</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Sensor not detected</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Czujnik temperatury nie działa</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Naprawiono</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Zewnętrzna ok</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Nie działa poprawnie cały czas widnieje Close</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Oderwany od framugi, ale działa poprawnie</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Jest, nie działa</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Działa poprawnie, ale jest odklejony</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Cały czas pokazuje Close</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Cały czas pokazuje Open</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Nie ma kontaktronu na drzwiach/drzwi nie da się zamknąć</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Brak kontaktronów w drzwiach</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>nie wykrywa otwarcia</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Brak przewodów do kontaktronu</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Lewy działa prawy nie da się otworzyć</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Nie działa poprawnie cały czas widnieje napis close</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Nie działa cały czas pokazuje Close</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Nie działa cały czas pokazuje Open</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Nie działa cały czas pokazuje Open (update)</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Nie działa</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Nie działa, close cały czas</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Nie ma jak sprawdzić, okna nie można zamknąć</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Były w excelu, ale działają</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Kontraktron skip</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Tylko jedno okno da się sprawdzić - działa, drugie jest za wysoko</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Na górnym oknie nie da się sprawdzić, za wysoko</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Cały czas pokazuje Open</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Okno</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Cały czas pisze close</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Nie działa ciągle pisze close</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Ciągle widnieje napis Close</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Nie można sprawdzić, nie da się otworzyć okna</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Kontaktronu podłączone równolegle zamiast szeregowo</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Ciągle pisze close</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Stan close cały czas</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Jedno okno działa prawidłowo, drugie zamknięte na klucz - nie można sprawdzić</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Kontaktron w oknie nie działa. Okno widnieje jako otwarte zawsze.</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Nie wykrywa otwarcia, sprawdzony miernikiem</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>nie działa</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Nie reaguje na zmianę stanu cały czas wykrywa napięcie</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić kuchenka nie włącza się</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Nie ma napięcia na przewodzie, nie pstryka</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Nie pstryka</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Nie reaguje na zmianę stanu cały czas wykrywa napięcie , voltage state not detected</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Nie działa zmiana ogrzewania</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>cały czas jest napięcie na przewodzie</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>nie załącza sie</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Voltage state not detected - brak napięcia na głowicy</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Nie słychać cykania przy zmianie, nie działa</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Kuchenki nie da się połączyć do gniazdka</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Kuchenki nie da się połączyć do gniazdka/nie da się sprawdzić</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Kuchenka nie włącza się nie słuchać pstrykania</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Kuchenka nie zmienia swojego stanu słychać pstrykanie</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić, brak wtyczki</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Nie jest podłączona nie da się sprawdzić</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić, kuchenka nie jest podłączona do prądu, za krótki przewod</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Podłączona do tego złego gniazdka, nie ma dojścia żeby zmienić, pstryka</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Gniazdko od kuchenki nie działa, kuchenka wogole się nie włącza na tym gniazdku</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Brak możliwości sprawdzenia, pomimo podłączenia do gniazdka nie włącza się, sprawdzane na dwóch gniazdkach, pstryka</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić przez brak możliwości wpięcia wtyczki</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Nie można sprawdzić funkcjonalności, źle podpięta, brak dostępu do gniazda</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Kuchenka nie włącza się nie słychać pstrykania</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Kuchenka się nie włącza nie słychać pstrykania</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Nie działa</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Nie działa kuchenka</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Nie dziala</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić nie jest podpięta do prądu</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić przez brak możliwości dostania się do kuchenki</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Nie da się sprawdzić brak napięcia w gniazdku</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Nie ma dostępu do gniazdka</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Niepoprawne ssid jest widoczne - 394-ED4. Poprawne to A3D-31F</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>zle ssid</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>złe ssid</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Small refactor and add analysis
</commit_message>
<xml_diff>
--- a/logs_analysis.xlsx
+++ b/logs_analysis.xlsx
@@ -1792,12 +1792,12 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -42286,12 +42286,12 @@
       </c>
       <c r="T607" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
       <c r="U607" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -45193,7 +45193,7 @@
       </c>
       <c r="U648" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -45333,7 +45333,7 @@
       </c>
       <c r="U650" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -45473,7 +45473,7 @@
       </c>
       <c r="U652" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -45613,7 +45613,7 @@
       </c>
       <c r="U654" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -46959,7 +46959,7 @@
       </c>
       <c r="U673" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -48877,7 +48877,7 @@
       </c>
       <c r="U700" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -50801,7 +50801,7 @@
       </c>
       <c r="U728" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -56083,7 +56083,7 @@
       </c>
       <c r="U803" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>
@@ -56218,12 +56218,12 @@
       </c>
       <c r="T805" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
       <c r="U805" t="inlineStr">
         <is>
-          <t>Brak danych</t>
+          <t>NO_DATA</t>
         </is>
       </c>
     </row>

</xml_diff>